<commit_message>
Added Sediment POC tab
</commit_message>
<xml_diff>
--- a/POC_Sediment_Samples.xlsx
+++ b/POC_Sediment_Samples.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efons\Desktop\POC_Sediment_Samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efons\eoa-webapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -61811,14 +61811,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N434"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="B415" workbookViewId="0">
+      <selection activeCell="D442" sqref="D442"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="240.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
     <col min="14" max="14" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -61920,6 +61922,9 @@
       <c r="C3" t="s">
         <v>950</v>
       </c>
+      <c r="D3" s="1">
+        <v>36892</v>
+      </c>
       <c r="E3">
         <v>37.412640000000003</v>
       </c>
@@ -62401,6 +62406,9 @@
       <c r="C14" t="s">
         <v>950</v>
       </c>
+      <c r="D14" s="1">
+        <v>36892</v>
+      </c>
       <c r="E14">
         <v>37.426049999999996</v>
       </c>
@@ -62574,6 +62582,9 @@
       <c r="C18" t="s">
         <v>950</v>
       </c>
+      <c r="D18" s="1">
+        <v>36892</v>
+      </c>
       <c r="E18">
         <v>37.424250000000001</v>
       </c>
@@ -62615,6 +62626,9 @@
       <c r="C19" t="s">
         <v>950</v>
       </c>
+      <c r="D19" s="1">
+        <v>36892</v>
+      </c>
       <c r="E19">
         <v>37.425020000000004</v>
       </c>
@@ -62964,6 +62978,9 @@
       <c r="C27" t="s">
         <v>950</v>
       </c>
+      <c r="D27" s="1">
+        <v>36892</v>
+      </c>
       <c r="E27">
         <v>37.40325</v>
       </c>
@@ -63093,6 +63110,9 @@
       <c r="C30" t="s">
         <v>950</v>
       </c>
+      <c r="D30" s="1">
+        <v>36892</v>
+      </c>
       <c r="E30">
         <v>37.428229999999999</v>
       </c>
@@ -63662,6 +63682,9 @@
       <c r="C43" t="s">
         <v>950</v>
       </c>
+      <c r="D43" s="1">
+        <v>36892</v>
+      </c>
       <c r="E43">
         <v>37.406579999999998</v>
       </c>
@@ -63879,6 +63902,9 @@
       <c r="C48" t="s">
         <v>950</v>
       </c>
+      <c r="D48" s="1">
+        <v>37257</v>
+      </c>
       <c r="E48">
         <v>37.403832999999999</v>
       </c>
@@ -63920,6 +63946,9 @@
       <c r="C49" t="s">
         <v>950</v>
       </c>
+      <c r="D49" s="1">
+        <v>37257</v>
+      </c>
       <c r="E49">
         <v>37.402233000000003</v>
       </c>
@@ -63961,6 +63990,9 @@
       <c r="C50" t="s">
         <v>950</v>
       </c>
+      <c r="D50" s="1">
+        <v>37257</v>
+      </c>
       <c r="E50">
         <v>37.401249999999997</v>
       </c>
@@ -64310,6 +64342,9 @@
       <c r="C58" t="s">
         <v>950</v>
       </c>
+      <c r="D58" s="1">
+        <v>36892</v>
+      </c>
       <c r="E58">
         <v>37.380879999999998</v>
       </c>
@@ -64571,6 +64606,9 @@
       <c r="C64" t="s">
         <v>950</v>
       </c>
+      <c r="D64" s="1">
+        <v>36892</v>
+      </c>
       <c r="E64">
         <v>37.375749999999996</v>
       </c>
@@ -65228,6 +65266,9 @@
       <c r="C79" t="s">
         <v>950</v>
       </c>
+      <c r="D79" s="1">
+        <v>36892</v>
+      </c>
       <c r="E79">
         <v>37.376370000000001</v>
       </c>
@@ -67601,6 +67642,9 @@
       <c r="C133" t="s">
         <v>950</v>
       </c>
+      <c r="D133" s="1">
+        <v>36892</v>
+      </c>
       <c r="E133">
         <v>37.36468</v>
       </c>
@@ -67818,6 +67862,9 @@
       <c r="C138" t="s">
         <v>950</v>
       </c>
+      <c r="D138" s="1">
+        <v>36892</v>
+      </c>
       <c r="E138">
         <v>37.370170000000002</v>
       </c>
@@ -70408,6 +70455,9 @@
       <c r="C197" t="s">
         <v>950</v>
       </c>
+      <c r="D197" s="1">
+        <v>36892</v>
+      </c>
       <c r="E197">
         <v>37.362029999999997</v>
       </c>
@@ -70977,6 +71027,9 @@
       <c r="C210" t="s">
         <v>950</v>
       </c>
+      <c r="D210" s="1">
+        <v>36892</v>
+      </c>
       <c r="E210">
         <v>37.34572</v>
       </c>
@@ -71722,6 +71775,9 @@
       <c r="C227" t="s">
         <v>950</v>
       </c>
+      <c r="D227" s="1">
+        <v>36892</v>
+      </c>
       <c r="E227">
         <v>37.345419999999997</v>
       </c>
@@ -72951,6 +73007,9 @@
       <c r="C255" t="s">
         <v>950</v>
       </c>
+      <c r="D255" s="1">
+        <v>37257</v>
+      </c>
       <c r="E255">
         <v>37.311149999999998</v>
       </c>
@@ -72992,6 +73051,9 @@
       <c r="C256" t="s">
         <v>950</v>
       </c>
+      <c r="D256" s="1">
+        <v>37257</v>
+      </c>
       <c r="E256">
         <v>37.311782999999998</v>
       </c>
@@ -73033,6 +73095,9 @@
       <c r="C257" t="s">
         <v>950</v>
       </c>
+      <c r="D257" s="1">
+        <v>37257</v>
+      </c>
       <c r="E257">
         <v>37.311500000000002</v>
       </c>
@@ -73074,6 +73139,9 @@
       <c r="C258" t="s">
         <v>950</v>
       </c>
+      <c r="D258" s="1">
+        <v>37257</v>
+      </c>
       <c r="E258">
         <v>37.310633000000003</v>
       </c>
@@ -73115,6 +73183,9 @@
       <c r="C259" t="s">
         <v>950</v>
       </c>
+      <c r="D259" s="1">
+        <v>37257</v>
+      </c>
       <c r="E259">
         <v>37.310316999999998</v>
       </c>
@@ -73156,6 +73227,9 @@
       <c r="C260" t="s">
         <v>950</v>
       </c>
+      <c r="D260" s="1">
+        <v>37257</v>
+      </c>
       <c r="E260">
         <v>37.310316999999998</v>
       </c>
@@ -73197,6 +73271,9 @@
       <c r="C261" t="s">
         <v>950</v>
       </c>
+      <c r="D261" s="1">
+        <v>37257</v>
+      </c>
       <c r="E261">
         <v>37.310783000000001</v>
       </c>
@@ -73238,6 +73315,9 @@
       <c r="C262" t="s">
         <v>950</v>
       </c>
+      <c r="D262" s="1">
+        <v>37257</v>
+      </c>
       <c r="E262">
         <v>37.310299999999998</v>
       </c>
@@ -73279,6 +73359,9 @@
       <c r="C263" t="s">
         <v>950</v>
       </c>
+      <c r="D263" s="1">
+        <v>36892</v>
+      </c>
       <c r="E263">
         <v>37.31268</v>
       </c>
@@ -74596,6 +74679,9 @@
       <c r="C293" t="s">
         <v>950</v>
       </c>
+      <c r="D293" s="1">
+        <v>36892</v>
+      </c>
       <c r="E293">
         <v>37.313617000000001</v>
       </c>
@@ -74637,6 +74723,9 @@
       <c r="C294" t="s">
         <v>950</v>
       </c>
+      <c r="D294" s="1">
+        <v>37257</v>
+      </c>
       <c r="E294">
         <v>37.319049999999997</v>
       </c>
@@ -75382,6 +75471,9 @@
       <c r="C311" t="s">
         <v>950</v>
       </c>
+      <c r="D311" s="1">
+        <v>37257</v>
+      </c>
       <c r="E311">
         <v>37.307749999999999</v>
       </c>
@@ -75467,6 +75559,9 @@
       <c r="C313" t="s">
         <v>950</v>
       </c>
+      <c r="D313" s="1">
+        <v>37257</v>
+      </c>
       <c r="E313">
         <v>37.305767000000003</v>
       </c>
@@ -75728,6 +75823,9 @@
       <c r="C319" t="s">
         <v>950</v>
       </c>
+      <c r="D319" s="1">
+        <v>37257</v>
+      </c>
       <c r="E319">
         <v>37.312399999999997</v>
       </c>
@@ -76074,6 +76172,9 @@
       <c r="C327" t="s">
         <v>950</v>
       </c>
+      <c r="D327" s="1">
+        <v>37257</v>
+      </c>
       <c r="E327">
         <v>37.309019999999997</v>
       </c>
@@ -76115,6 +76216,9 @@
       <c r="C328" t="s">
         <v>950</v>
       </c>
+      <c r="D328" s="1">
+        <v>36892</v>
+      </c>
       <c r="E328">
         <v>37.309019999999997</v>
       </c>
@@ -76376,6 +76480,9 @@
       <c r="C334" t="s">
         <v>950</v>
       </c>
+      <c r="D334" s="1">
+        <v>36892</v>
+      </c>
       <c r="E334">
         <v>37.321060000000003</v>
       </c>
@@ -76417,6 +76524,9 @@
       <c r="C335" t="s">
         <v>950</v>
       </c>
+      <c r="D335" s="1">
+        <v>36892</v>
+      </c>
       <c r="E335">
         <v>37.317810000000001</v>
       </c>
@@ -76502,6 +76612,9 @@
       <c r="C337" t="s">
         <v>950</v>
       </c>
+      <c r="D337" s="1">
+        <v>36892</v>
+      </c>
       <c r="E337">
         <v>37.31033</v>
       </c>
@@ -77819,6 +77932,9 @@
       <c r="C367" t="s">
         <v>950</v>
       </c>
+      <c r="D367" s="1">
+        <v>36892</v>
+      </c>
       <c r="E367">
         <v>37.27178</v>
       </c>
@@ -77992,6 +78108,9 @@
       <c r="C371" t="s">
         <v>950</v>
       </c>
+      <c r="D371" s="1">
+        <v>36892</v>
+      </c>
       <c r="E371">
         <v>37.234810000000003</v>
       </c>
@@ -78077,6 +78196,9 @@
       <c r="C373" t="s">
         <v>950</v>
       </c>
+      <c r="D373" s="1">
+        <v>36892</v>
+      </c>
       <c r="E373">
         <v>37.418109999999999</v>
       </c>
@@ -78118,6 +78240,9 @@
       <c r="C374" t="s">
         <v>950</v>
       </c>
+      <c r="D374" s="1">
+        <v>36892</v>
+      </c>
       <c r="E374">
         <v>37.414830000000002</v>
       </c>
@@ -78203,6 +78328,9 @@
       <c r="C376" t="s">
         <v>950</v>
       </c>
+      <c r="D376" s="1">
+        <v>37257</v>
+      </c>
       <c r="E376">
         <v>37.404440000000001</v>
       </c>
@@ -78244,6 +78372,9 @@
       <c r="C377" t="s">
         <v>950</v>
       </c>
+      <c r="D377" s="1">
+        <v>36892</v>
+      </c>
       <c r="E377">
         <v>37.404440000000001</v>
       </c>
@@ -78285,6 +78416,9 @@
       <c r="C378" t="s">
         <v>950</v>
       </c>
+      <c r="D378" s="1">
+        <v>36892</v>
+      </c>
       <c r="E378">
         <v>37.404440000000001</v>
       </c>
@@ -78414,6 +78548,9 @@
       <c r="C381" t="s">
         <v>950</v>
       </c>
+      <c r="D381" s="1">
+        <v>36892</v>
+      </c>
       <c r="E381">
         <v>37.32011</v>
       </c>
@@ -78675,6 +78812,9 @@
       <c r="C387" t="s">
         <v>950</v>
       </c>
+      <c r="D387" s="1">
+        <v>36892</v>
+      </c>
       <c r="E387">
         <v>37.283650000000002</v>
       </c>
@@ -78716,6 +78856,9 @@
       <c r="C388" t="s">
         <v>950</v>
       </c>
+      <c r="D388" s="1">
+        <v>36892</v>
+      </c>
       <c r="E388">
         <v>37.421810000000001</v>
       </c>
@@ -78757,6 +78900,9 @@
       <c r="C389" t="s">
         <v>950</v>
       </c>
+      <c r="D389" s="1">
+        <v>36892</v>
+      </c>
       <c r="E389">
         <v>37.406480000000002</v>
       </c>
@@ -78930,6 +79076,9 @@
       <c r="C393" t="s">
         <v>950</v>
       </c>
+      <c r="D393" s="1">
+        <v>36892</v>
+      </c>
       <c r="E393">
         <v>37.415819999999997</v>
       </c>
@@ -79147,6 +79296,9 @@
       <c r="C398" t="s">
         <v>950</v>
       </c>
+      <c r="D398" s="1">
+        <v>36892</v>
+      </c>
       <c r="E398">
         <v>37.26144</v>
       </c>
@@ -79232,6 +79384,9 @@
       <c r="C400" t="s">
         <v>950</v>
       </c>
+      <c r="D400" s="1">
+        <v>36892</v>
+      </c>
       <c r="E400">
         <v>37.429549999999999</v>
       </c>
@@ -79537,6 +79692,9 @@
       <c r="C407" t="s">
         <v>950</v>
       </c>
+      <c r="D407" s="1">
+        <v>36892</v>
+      </c>
       <c r="E407">
         <v>37.268859999999997</v>
       </c>
@@ -79622,6 +79780,9 @@
       <c r="C409" t="s">
         <v>950</v>
       </c>
+      <c r="D409" s="1">
+        <v>36892</v>
+      </c>
       <c r="E409">
         <v>37.09939</v>
       </c>
@@ -79663,6 +79824,9 @@
       <c r="C410" t="s">
         <v>950</v>
       </c>
+      <c r="D410" s="1">
+        <v>36892</v>
+      </c>
       <c r="E410">
         <v>37.347070000000002</v>
       </c>
@@ -79704,6 +79868,9 @@
       <c r="C411" t="s">
         <v>950</v>
       </c>
+      <c r="D411" s="1">
+        <v>36892</v>
+      </c>
       <c r="E411">
         <v>37.388080000000002</v>
       </c>
@@ -80097,6 +80264,9 @@
       <c r="C420" t="s">
         <v>950</v>
       </c>
+      <c r="D420" s="1">
+        <v>36892</v>
+      </c>
       <c r="E420">
         <v>37.414470000000001</v>
       </c>
@@ -80138,6 +80308,9 @@
       <c r="C421" t="s">
         <v>950</v>
       </c>
+      <c r="D421" s="1">
+        <v>36892</v>
+      </c>
       <c r="E421">
         <v>37.40137</v>
       </c>
@@ -80354,6 +80527,9 @@
       </c>
       <c r="C426" t="s">
         <v>950</v>
+      </c>
+      <c r="D426" s="1">
+        <v>36892</v>
       </c>
       <c r="E426">
         <v>37.313870000000001</v>

</xml_diff>